<commit_message>
Result to xlsx new changes
</commit_message>
<xml_diff>
--- a/src/sample/JustOneSample/SimpleSampleCode.xlsx
+++ b/src/sample/JustOneSample/SimpleSampleCode.xlsx
@@ -12,18 +12,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">File name: </t>
   </si>
   <si>
-    <t>C:\Users\Danilo\Documents\GitHub\crowd-debug-firefly\src\sample\JustOneSample\SimpleSampleCode</t>
+    <t>SimpleSampleCode</t>
   </si>
   <si>
     <t xml:space="preserve">Number of Snippets: </t>
-  </si>
-  <si>
-    <t>put number here</t>
   </si>
   <si>
     <t xml:space="preserve">Number of questions: </t>
@@ -92,24 +89,24 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="B4" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Xlsx now with tabs
</commit_message>
<xml_diff>
--- a/src/sample/JustOneSample/SimpleSampleCode.xlsx
+++ b/src/sample/JustOneSample/SimpleSampleCode.xlsx
@@ -6,13 +6,52 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sumary" r:id="rId3" sheetId="1"/>
+    <sheet name="Summary" r:id="rId3" sheetId="1"/>
+    <sheet name="SeedVerifier" r:id="rId4" sheetId="2"/>
+    <sheet name="newCases" r:id="rId5" sheetId="3"/>
+    <sheet name="factorial" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Is there perhaps something wrong with the values of the parameters received by function 'intValue' when called by function 'SeedVerifier' at line 9 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Is there possibly something wrong with the body of function 'SeedVerifier' between lines 7 and 18 (e.g., function produces an incorrect return value, return statement is at the wrong place, does not properly handle error situations, etc.)?</t>
+  </si>
+  <si>
+    <t>PROBABLY_NOT</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong in the declaration of function 'SeedVerifier' at line 7 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause at line 8 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>PROBABLY_YES</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 8 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>I_CANT_TELL</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong in the declaration of function 'newCases' at line 32 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong in the declaration of function 'factorial' at line 20 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
+  </si>
   <si>
     <t xml:space="preserve">File name: </t>
   </si>
@@ -23,10 +62,10 @@
     <t xml:space="preserve">Number of Snippets: </t>
   </si>
   <si>
-    <t xml:space="preserve">Number of questions: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of statements: </t>
+    <t xml:space="preserve">Total number of questions: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of answers: </t>
   </si>
 </sst>
 </file>
@@ -76,18 +115,22 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
+  <cols>
+    <col min="1" max="1" width="25.73046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="18.1484375" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
         <v>3.0</v>
@@ -95,20 +138,141 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="208.0390625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2"/>
+    </row>
+    <row r="3"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="206.5546875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2"/>
+    </row>
+    <row r="3"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
New Method Data with ArrayList
</commit_message>
<xml_diff>
--- a/src/sample/JustOneSample/SimpleSampleCode.xlsx
+++ b/src/sample/JustOneSample/SimpleSampleCode.xlsx
@@ -15,42 +15,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 14 and 17 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 10 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
   <si>
     <t>Is there perhaps something wrong with the values of the parameters received by function 'intValue' when called by function 'SeedVerifier' at line 9 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Is there possibly something wrong with the body of function 'SeedVerifier' between lines 7 and 18 (e.g., function produces an incorrect return value, return statement is at the wrong place, does not properly handle error situations, etc.)?</t>
   </si>
   <si>
-    <t>PROBABLY_NOT</t>
+    <t>Is there maybe something wrong with the body of the conditional clause at line 12 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
   </si>
   <si>
     <t>Is there maybe something wrong in the declaration of function 'SeedVerifier' at line 7 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
   </si>
   <si>
-    <t>NO</t>
+    <t>Is there maybe something wrong with the body of the conditional clause at line 11 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 13 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
   </si>
   <si>
     <t>Is there maybe something wrong with the body of the conditional clause at line 8 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
   </si>
   <si>
-    <t>PROBABLY_YES</t>
-  </si>
-  <si>
     <t>Is it possible that the conditional clause at line 8 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
   </si>
   <si>
-    <t>I_CANT_TELL</t>
+    <t>Is it possible that the conditional clause at line 12 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 59 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'Do-loop' between lines 88 and 91 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 68 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'For-loop' construct at line 61 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 59 and 79 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 60 and 75 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 77 and 79 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'Do-loop' construct at line 97 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there possibly something wrong with the body of function 'newCases' between lines 32 and 110 (e.g., function produces an incorrect return value, return statement is at the wrong place, does not properly handle error situations, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 77 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'For-loop' between lines 61 and 64 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'Do-loop' between lines 82 and 86 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'For-loop' between lines 55 and 80 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 102 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 102 and 109 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'For-loop' at line 53 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'Do-loop' construct at line 87 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 98 and 101 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 35 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'Do-loop' construct at line 92 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
   </si>
   <si>
     <t>Is there maybe something wrong in the declaration of function 'newCases' at line 32 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
   </si>
   <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 37 and 50 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'For-loop' construct at line 52 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there perhaps something wrong with the values of the parameters received by function 'factorial' when called by function 'newCases' at line 84 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 69 and 75 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there perhaps something wrong with the values of the parameters received by function 'toString' when called by function 'newCases' at line 53 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 66 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 98 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 67 and 75 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'Do-loop' between lines 93 and 96 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 60 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'For-loop' construct at line 55 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there perhaps something wrong with the values of the parameters received by function 'intValue' when called by function 'factorial' at line 23 (e.g., wrong variables used as parameters, wrong order, missing or wrong type of parameter, values of the parameters are not checked, etc .)?</t>
+  </si>
+  <si>
     <t>Is there maybe something wrong in the declaration of function 'factorial' at line 20 (e.g., requires a parameter that is not listed, needs different parameters to produce the correct result, specifies the wrong or no return type, etc .)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the 'For-loop' construct at line 23 (e.g., incorrect initialization, wrong counter increment, wrong exit condition, etc.)?</t>
+  </si>
+  <si>
+    <t>Is it possible that the conditional clause at line 21 has problems (e.g., wrong Boolean operator, wrong comparison, misplaced parentheses, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there possibly something wrong with the body of function 'factorial' between lines 20 and 30 (e.g., function produces an incorrect return value, return statement is at the wrong place, does not properly handle error situations, etc.)?</t>
+  </si>
+  <si>
+    <t>Is there maybe something wrong with the body of the conditional clause between lines 22 and 29 (e.g., enters the wrong branch, makes a call to a null pointer, calls a wrong type, etc.)?</t>
+  </si>
+  <si>
+    <t>Is the body of the 'For-loop' between lines 23 and 25 possibly not producing what it is supposed to (e.g., does not compute the expected result, does not exit at the expected iteration, etc.)?</t>
   </si>
   <si>
     <t xml:space="preserve">File name: </t>
@@ -122,15 +236,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B2" t="n">
         <v>3.0</v>
@@ -138,18 +252,18 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B3" t="n">
-        <v>7.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B4" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -174,55 +288,99 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2"/>
     </row>
     <row r="3"/>
     <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5"/>
     </row>
     <row r="6"/>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
+      <c r="A8"/>
     </row>
     <row r="9"/>
     <row r="10">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11"/>
     </row>
     <row r="12"/>
     <row r="13">
       <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+    </row>
+    <row r="21"/>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+    </row>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
+    <row r="26">
+      <c r="A26"/>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15"/>
+    <row r="29">
+      <c r="A29"/>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32"/>
+    </row>
+    <row r="33"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -236,18 +394,297 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="208.0390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2"/>
     </row>
     <row r="3"/>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+    </row>
+    <row r="21"/>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+    </row>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26"/>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29"/>
+    </row>
+    <row r="30"/>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32"/>
+    </row>
+    <row r="33"/>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35"/>
+    </row>
+    <row r="36"/>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38"/>
+    </row>
+    <row r="39"/>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41"/>
+    </row>
+    <row r="42"/>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44"/>
+    </row>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47"/>
+    </row>
+    <row r="48"/>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50"/>
+    </row>
+    <row r="51"/>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+    </row>
+    <row r="54"/>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56"/>
+    </row>
+    <row r="57"/>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59"/>
+    </row>
+    <row r="60"/>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+    </row>
+    <row r="63"/>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+    </row>
+    <row r="66"/>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68"/>
+    </row>
+    <row r="69"/>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71"/>
+    </row>
+    <row r="72"/>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74"/>
+    </row>
+    <row r="75"/>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77"/>
+    </row>
+    <row r="78"/>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80"/>
+    </row>
+    <row r="81"/>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83"/>
+    </row>
+    <row r="84"/>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86"/>
+    </row>
+    <row r="87"/>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89"/>
+    </row>
+    <row r="90"/>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92"/>
+    </row>
+    <row r="93"/>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95"/>
+    </row>
+    <row r="96"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -261,18 +698,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="206.5546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
       <c r="A2"/>
     </row>
     <row r="3"/>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+    </row>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+    </row>
+    <row r="15"/>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+    </row>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+    </row>
+    <row r="21"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>